<commit_message>
updated with datadriven approch for testing multiple set of data
</commit_message>
<xml_diff>
--- a/OnNativeWebHybridApplication/src/test/java/com/config/mobiletestinglogins.xlsx
+++ b/OnNativeWebHybridApplication/src/test/java/com/config/mobiletestinglogins.xlsx
@@ -1,24 +1,24 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="23628"/>
   <workbookPr/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+  <mc:AlternateContent>
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\DuvarakeshKV\Desktop\reskill\MOBILE TESTING\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\DuvarakeshKV\Mobile_testing\OnNativeWebHybridApplication\src\test\java\com\config\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AB8B9F16-2BFD-439A-BECA-A1B6B023481A}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr documentId="13_ncr:1_{2F648ED5-178E-47DB-B466-10A25D4521CE}" revIDLastSave="0" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10560" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView windowHeight="10560" windowWidth="19420" xWindow="-110" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}" yWindow="-110"/>
   </bookViews>
   <sheets>
-    <sheet name="DATA_SHEET" sheetId="2" r:id="rId1"/>
-    <sheet name="OUTPUT_DATASHEET" sheetId="3" r:id="rId2"/>
+    <sheet name="DATA_SHEET" r:id="rId1" sheetId="2"/>
+    <sheet name="OUTPUT_DATASHEET" r:id="rId2" sheetId="3"/>
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
+    <ext uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
   </extLst>
@@ -49,9 +49,6 @@
     <t>VENUGOPAL</t>
   </si>
   <si>
-    <t>DUVARAKESH123@GMAIL.COM</t>
-  </si>
-  <si>
     <t>DUVA12345</t>
   </si>
   <si>
@@ -100,22 +97,26 @@
     <t>ACTUAL_OUTPUT</t>
   </si>
   <si>
+    <t>EXPECTED OUTPUT</t>
+  </si>
+  <si>
+    <t>STATUS</t>
+  </si>
+  <si>
+    <t>DUVAKSH123@GMAIL.COM</t>
+  </si>
+  <si>
+    <t>AR321882@GMAIL.COM</t>
+  </si>
+  <si>
     <t>PASSED</t>
-  </si>
-  <si>
-    <t>EXPECTED OUTPUT</t>
-  </si>
-  <si>
-    <t>STATUS</t>
-  </si>
-  <si>
-    <t>DUVAR3212@GMAIL.COM</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <numFmts count="0"/>
   <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -169,22 +170,22 @@
     </border>
   </borders>
   <cellStyleXfs count="2">
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0"/>
+    <xf applyAlignment="0" applyBorder="0" applyFill="0" applyNumberFormat="0" applyProtection="0" borderId="0" fillId="0" fontId="1" numFmtId="0"/>
   </cellStyleXfs>
   <cellXfs count="5">
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
+    <xf borderId="0" fillId="0" fontId="1" numFmtId="0" xfId="1"/>
+    <xf applyFill="1" borderId="0" fillId="2" fontId="0" numFmtId="0" xfId="0"/>
+    <xf applyFill="1" borderId="0" fillId="3" fontId="0" numFmtId="0" xfId="0"/>
+    <xf applyFill="1" borderId="0" fillId="4" fontId="0" numFmtId="0" xfId="0"/>
   </cellXfs>
   <cellStyles count="2">
-    <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
-    <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle builtinId="8" name="Hyperlink" xfId="1"/>
+    <cellStyle builtinId="0" name="Normal" xfId="0"/>
   </cellStyles>
   <dxfs count="0"/>
-  <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
+  <tableStyles count="0" defaultPivotStyle="PivotStyleLight16" defaultTableStyle="TableStyleMedium2"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
@@ -201,10 +202,10 @@
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
-        <a:sysClr val="windowText" lastClr="000000"/>
+        <a:sysClr lastClr="000000" val="windowText"/>
       </a:dk1>
       <a:lt1>
-        <a:sysClr val="window" lastClr="FFFFFF"/>
+        <a:sysClr lastClr="FFFFFF" val="window"/>
       </a:lt1>
       <a:dk2>
         <a:srgbClr val="44546A"/>
@@ -239,7 +240,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
+        <a:latin panose="020F0302020204030204" typeface="Calibri Light"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="游ゴシック Light"/>
@@ -274,7 +275,7 @@
         <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+        <a:latin panose="020F0502020204030204" typeface="Calibri"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="游ゴシック"/>
@@ -368,21 +369,21 @@
         </a:gradFill>
       </a:fillStyleLst>
       <a:lnStyleLst>
-        <a:ln w="6350" cap="flat" cmpd="sng" algn="ctr">
+        <a:ln algn="ctr" cap="flat" cmpd="sng" w="6350">
           <a:solidFill>
             <a:schemeClr val="phClr"/>
           </a:solidFill>
           <a:prstDash val="solid"/>
           <a:miter lim="800000"/>
         </a:ln>
-        <a:ln w="12700" cap="flat" cmpd="sng" algn="ctr">
+        <a:ln algn="ctr" cap="flat" cmpd="sng" w="12700">
           <a:solidFill>
             <a:schemeClr val="phClr"/>
           </a:solidFill>
           <a:prstDash val="solid"/>
           <a:miter lim="800000"/>
         </a:ln>
-        <a:ln w="19050" cap="flat" cmpd="sng" algn="ctr">
+        <a:ln algn="ctr" cap="flat" cmpd="sng" w="19050">
           <a:solidFill>
             <a:schemeClr val="phClr"/>
           </a:solidFill>
@@ -399,7 +400,7 @@
         </a:effectStyle>
         <a:effectStyle>
           <a:effectLst>
-            <a:outerShdw blurRad="57150" dist="19050" dir="5400000" algn="ctr" rotWithShape="0">
+            <a:outerShdw algn="ctr" blurRad="57150" dir="5400000" dist="19050" rotWithShape="0">
               <a:srgbClr val="000000">
                 <a:alpha val="63000"/>
               </a:srgbClr>
@@ -451,26 +452,26 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" name="Office Theme" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E4F5CFD9-5679-4AF9-9CF8-045E44CEDBA2}">
-  <dimension ref="A1:H5"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E4F5CFD9-5679-4AF9-9CF8-045E44CEDBA2}">
+  <dimension ref="A1:I5"/>
   <sheetViews>
-    <sheetView topLeftCell="C1" workbookViewId="0">
-      <selection activeCell="F10" sqref="F10"/>
+    <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
+      <selection activeCell="C5" sqref="C5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="17.26953125" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="3" max="3" width="30.36328125" customWidth="1" collapsed="1"/>
-    <col min="5" max="5" width="22.36328125" customWidth="1" collapsed="1"/>
-    <col min="6" max="6" width="54.453125" customWidth="1" collapsed="1"/>
-    <col min="7" max="7" width="22.36328125" customWidth="1" collapsed="1"/>
+    <col min="3" max="3" customWidth="true" width="30.36328125" collapsed="true"/>
+    <col min="5" max="5" customWidth="true" width="22.36328125" collapsed="true"/>
+    <col min="6" max="6" customWidth="true" width="54.453125" collapsed="true"/>
+    <col min="7" max="7" customWidth="true" width="22.36328125" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:8" x14ac:dyDescent="0.35">
@@ -490,7 +491,7 @@
         <v>4</v>
       </c>
       <c r="F1" s="2" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="G1" s="4"/>
       <c r="H1" s="4"/>
@@ -503,159 +504,159 @@
         <v>6</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>7</v>
+        <v>25</v>
       </c>
       <c r="D2" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="E2" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="F2" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
+        <v>9</v>
+      </c>
+      <c r="B3" t="s">
+        <v>8</v>
+      </c>
+      <c r="C3" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="B3" t="s">
-        <v>9</v>
-      </c>
-      <c r="C3" s="1" t="s">
+      <c r="D3" t="s">
+        <v>7</v>
+      </c>
+      <c r="E3" t="s">
         <v>11</v>
       </c>
-      <c r="D3" t="s">
-        <v>8</v>
-      </c>
-      <c r="E3" t="s">
-        <v>12</v>
-      </c>
       <c r="F3" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
+        <v>18</v>
+      </c>
+      <c r="B4" t="s">
         <v>19</v>
       </c>
-      <c r="B4" t="s">
-        <v>20</v>
-      </c>
       <c r="C4" s="1" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="D4" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="E4" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="F4" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
     </row>
     <row r="5" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
+        <v>20</v>
+      </c>
+      <c r="B5" t="s">
         <v>21</v>
       </c>
-      <c r="B5" t="s">
-        <v>22</v>
-      </c>
       <c r="C5" s="1" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="D5" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="E5" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="F5" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="C2" r:id="rId1" xr:uid="{0F95653F-2E3C-4E6E-AE64-DAFD373841F3}"/>
-    <hyperlink ref="C3" r:id="rId2" xr:uid="{320C0267-0EFA-4254-84D3-C1FC2581F190}"/>
-    <hyperlink ref="C4" r:id="rId3" display="DUVARAKESH123@GMAIL.COM" xr:uid="{0DED0194-91F5-49FC-99FB-002F3C9FD054}"/>
-    <hyperlink ref="C5" r:id="rId4" xr:uid="{1087DC51-FA85-4E04-8331-937D0BB4B8ED}"/>
+    <hyperlink r:id="rId1" ref="C2" xr:uid="{0F95653F-2E3C-4E6E-AE64-DAFD373841F3}"/>
+    <hyperlink r:id="rId2" ref="C3" xr:uid="{320C0267-0EFA-4254-84D3-C1FC2581F190}"/>
+    <hyperlink display="DUVARAKESH123@GMAIL.COM" r:id="rId3" ref="C4" xr:uid="{0DED0194-91F5-49FC-99FB-002F3C9FD054}"/>
+    <hyperlink r:id="rId4" ref="C5" xr:uid="{1087DC51-FA85-4E04-8331-937D0BB4B8ED}"/>
   </hyperlinks>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F816D599-DC9B-4D05-B3D3-B8D15113ACAB}">
-  <dimension ref="A1:C5"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F816D599-DC9B-4D05-B3D3-B8D15113ACAB}">
+  <dimension ref="A1:D5"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A9" sqref="A9"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A10" sqref="A10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="59" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="49.7265625" customWidth="1" collapsed="1"/>
+    <col min="1" max="1" customWidth="true" width="59.0" collapsed="true"/>
+    <col min="2" max="2" customWidth="true" width="49.7265625" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A1" s="3" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="B1" s="3" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="C1" s="3" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.35">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="2">
       <c r="A2" t="s">
+        <v>14</v>
+      </c>
+      <c r="B2" t="s">
+        <v>14</v>
+      </c>
+      <c r="C2" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" t="s">
         <v>15</v>
       </c>
-      <c r="B2" t="s">
+      <c r="B3" t="s">
         <v>15</v>
       </c>
-      <c r="C2" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A3" t="s">
+      <c r="C3" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" t="s">
         <v>16</v>
       </c>
-      <c r="B3" t="s">
+      <c r="B4" t="s">
         <v>16</v>
       </c>
-      <c r="C3" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A4" t="s">
-        <v>17</v>
-      </c>
-      <c r="B4" t="s">
-        <v>17</v>
-      </c>
       <c r="C4" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.35">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="5">
       <c r="A5" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="B5" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="C5" t="s">
-        <v>24</v>
+        <v>27</v>
       </c>
     </row>
   </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
 </worksheet>
 </file>
</xml_diff>